<commit_message>
TRA2501 template change (hyperlinks)
</commit_message>
<xml_diff>
--- a/inst/TRA2501_template.xlsx
+++ b/inst/TRA2501_template.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\virago.internal.dtlr.gov.uk\u\Lon1\LSHAW\My Documents\Keep Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LukeS\Documents\ac-roadtraff-pipe\inst\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -45,13 +45,13 @@
     <definedName name="fendyear">[2]Year!$B$3</definedName>
     <definedName name="FOREIGN">[1]TABLE1a!$P$38:$P$52</definedName>
     <definedName name="fyear">[2]c11!$D$42</definedName>
-    <definedName name="GraphData">'[4]TIS-INDEX'!$B$13:$Q$44,'[4]TIS-INDEX'!$E$9:$R$9</definedName>
+    <definedName name="GraphData">'[3]TIS-INDEX'!$B$13:$Q$44,'[3]TIS-INDEX'!$E$9:$R$9</definedName>
     <definedName name="LGV_data">!#REF!</definedName>
     <definedName name="Print_Area_MI">[1]TABLE1a!$A$1:$O$37</definedName>
-    <definedName name="tab" localSheetId="0">[3]TABLE1a!$U$3</definedName>
-    <definedName name="tab">[3]TABLE1a!$U$3</definedName>
+    <definedName name="tab" localSheetId="0">[4]TABLE1a!$U$3</definedName>
+    <definedName name="tab">[4]TABLE1a!$U$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -142,11 +142,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -247,7 +247,13 @@
     <font>
       <u/>
       <sz val="12"/>
-      <color theme="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -284,7 +290,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
@@ -318,11 +324,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="6" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
@@ -358,7 +366,13 @@
     <xdr:ext cx="847721" cy="723903"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 1"/>
+        <xdr:cNvPr id="3" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -396,7 +410,13 @@
     <xdr:ext cx="1542857" cy="1009525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 3"/>
+        <xdr:cNvPr id="2" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -474,6 +494,9 @@
       <sheetName val="FiguresSA_-do_not_print13"/>
       <sheetName val="TABLE2cont__14"/>
       <sheetName val="FiguresSA_-do_not_print14"/>
+      <sheetName val="Year"/>
+      <sheetName val="c11"/>
+      <sheetName val="TIS-INDEX"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0"/>
@@ -617,21 +640,15 @@
           <cell r="I11">
             <v>5.8</v>
           </cell>
-          <cell r="J11" t="str">
-            <v/>
-          </cell>
+          <cell r="J11"/>
           <cell r="K11">
             <v>796.2</v>
           </cell>
-          <cell r="L11" t="str">
-            <v/>
-          </cell>
+          <cell r="L11"/>
           <cell r="M11">
             <v>539.4</v>
           </cell>
-          <cell r="N11" t="str">
-            <v/>
-          </cell>
+          <cell r="N11"/>
           <cell r="O11">
             <v>1335.6</v>
           </cell>
@@ -649,21 +666,15 @@
           <cell r="I12">
             <v>4</v>
           </cell>
-          <cell r="J12" t="str">
-            <v/>
-          </cell>
+          <cell r="J12"/>
           <cell r="K12">
             <v>896.5</v>
           </cell>
-          <cell r="L12" t="str">
-            <v/>
-          </cell>
+          <cell r="L12"/>
           <cell r="M12">
             <v>701.6</v>
           </cell>
-          <cell r="N12" t="str">
-            <v/>
-          </cell>
+          <cell r="N12"/>
           <cell r="O12">
             <v>1598.1</v>
           </cell>
@@ -1384,6 +1395,9 @@
       <sheetData sheetId="41"/>
       <sheetData sheetId="42"/>
       <sheetData sheetId="43"/>
+      <sheetData sheetId="44" refreshError="1"/>
+      <sheetData sheetId="45" refreshError="1"/>
+      <sheetData sheetId="46" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1604,6 +1618,1111 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
+      <sheetName val="TIS-INDEX"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="9">
+          <cell r="E9">
+            <v>1983</v>
+          </cell>
+          <cell r="F9">
+            <v>1984</v>
+          </cell>
+          <cell r="G9">
+            <v>1985</v>
+          </cell>
+          <cell r="H9">
+            <v>1986</v>
+          </cell>
+          <cell r="I9">
+            <v>1987</v>
+          </cell>
+          <cell r="J9">
+            <v>1988</v>
+          </cell>
+          <cell r="K9">
+            <v>1989</v>
+          </cell>
+          <cell r="L9">
+            <v>1990</v>
+          </cell>
+          <cell r="M9">
+            <v>1991</v>
+          </cell>
+          <cell r="N9">
+            <v>1992</v>
+          </cell>
+          <cell r="O9">
+            <v>1993</v>
+          </cell>
+          <cell r="P9">
+            <v>1994</v>
+          </cell>
+          <cell r="Q9">
+            <v>1995</v>
+          </cell>
+          <cell r="R9">
+            <v>1996</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="B13" t="str">
+            <v>Road 1</v>
+          </cell>
+          <cell r="E13">
+            <v>4.2</v>
+          </cell>
+          <cell r="F13">
+            <v>4</v>
+          </cell>
+          <cell r="G13">
+            <v>4.3</v>
+          </cell>
+          <cell r="H13">
+            <v>3.7</v>
+          </cell>
+          <cell r="I13">
+            <v>4.0999999999999996</v>
+          </cell>
+          <cell r="J13">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="K13">
+            <v>4.5</v>
+          </cell>
+          <cell r="L13">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="M13">
+            <v>4.9000000000000004</v>
+          </cell>
+          <cell r="N13">
+            <v>4.5</v>
+          </cell>
+          <cell r="O13">
+            <v>5</v>
+          </cell>
+          <cell r="P13">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="Q13">
+            <v>5.7</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v xml:space="preserve">Rail </v>
+          </cell>
+          <cell r="E14">
+            <v>2.2999999999999998</v>
+          </cell>
+          <cell r="F14">
+            <v>2.2000000000000002</v>
+          </cell>
+          <cell r="G14">
+            <v>2</v>
+          </cell>
+          <cell r="H14">
+            <v>2.1</v>
+          </cell>
+          <cell r="I14">
+            <v>2</v>
+          </cell>
+          <cell r="J14">
+            <v>2.2000000000000002</v>
+          </cell>
+          <cell r="K14">
+            <v>2.2000000000000002</v>
+          </cell>
+          <cell r="L14">
+            <v>2.1</v>
+          </cell>
+          <cell r="M14">
+            <v>2</v>
+          </cell>
+          <cell r="N14">
+            <v>2</v>
+          </cell>
+          <cell r="O14">
+            <v>1.91</v>
+          </cell>
+          <cell r="P14">
+            <v>1.8220000000000001</v>
+          </cell>
+          <cell r="Q14">
+            <v>1.7</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v xml:space="preserve">Water </v>
+          </cell>
+          <cell r="E15">
+            <v>51.4</v>
+          </cell>
+          <cell r="F15">
+            <v>53.1</v>
+          </cell>
+          <cell r="G15">
+            <v>50.9</v>
+          </cell>
+          <cell r="H15">
+            <v>46</v>
+          </cell>
+          <cell r="I15">
+            <v>43.9</v>
+          </cell>
+          <cell r="J15">
+            <v>49.3</v>
+          </cell>
+          <cell r="K15">
+            <v>47.9</v>
+          </cell>
+          <cell r="L15">
+            <v>45.4</v>
+          </cell>
+          <cell r="M15">
+            <v>46</v>
+          </cell>
+          <cell r="N15">
+            <v>42.7</v>
+          </cell>
+          <cell r="O15">
+            <v>41.7</v>
+          </cell>
+          <cell r="P15">
+            <v>43</v>
+          </cell>
+          <cell r="Q15">
+            <v>42.5</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="B16" t="str">
+            <v>ow:  coastwise</v>
+          </cell>
+          <cell r="E16">
+            <v>40.200000000000003</v>
+          </cell>
+          <cell r="F16">
+            <v>41</v>
+          </cell>
+          <cell r="G16">
+            <v>38.9</v>
+          </cell>
+          <cell r="H16">
+            <v>33.9</v>
+          </cell>
+          <cell r="I16">
+            <v>31.4</v>
+          </cell>
+          <cell r="J16">
+            <v>34.200000000000003</v>
+          </cell>
+          <cell r="K16">
+            <v>34.1</v>
+          </cell>
+          <cell r="L16">
+            <v>32.1</v>
+          </cell>
+          <cell r="M16">
+            <v>31.2</v>
+          </cell>
+          <cell r="N16">
+            <v>29.4</v>
+          </cell>
+          <cell r="O16">
+            <v>28.9</v>
+          </cell>
+          <cell r="P16">
+            <v>28.9</v>
+          </cell>
+          <cell r="Q16">
+            <v>31.4</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="B17" t="str">
+            <v xml:space="preserve">Pipeline </v>
+          </cell>
+          <cell r="H17">
+            <v>10.4</v>
+          </cell>
+          <cell r="I17">
+            <v>10.5</v>
+          </cell>
+          <cell r="J17">
+            <v>11.1</v>
+          </cell>
+          <cell r="K17">
+            <v>9.8000000000000007</v>
+          </cell>
+          <cell r="L17">
+            <v>11.1</v>
+          </cell>
+          <cell r="M17">
+            <v>11.1</v>
+          </cell>
+          <cell r="N17">
+            <v>11</v>
+          </cell>
+          <cell r="O17">
+            <v>11.6</v>
+          </cell>
+          <cell r="P17">
+            <v>12</v>
+          </cell>
+          <cell r="Q17">
+            <v>12.2</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="B18" t="str">
+            <v>Pipeline</v>
+          </cell>
+          <cell r="E18">
+            <v>9.9</v>
+          </cell>
+          <cell r="F18">
+            <v>10.4</v>
+          </cell>
+          <cell r="G18">
+            <v>11.2</v>
+          </cell>
+          <cell r="H18">
+            <v>10.4</v>
+          </cell>
+          <cell r="I18">
+            <v>10.5</v>
+          </cell>
+          <cell r="J18">
+            <v>11.1</v>
+          </cell>
+          <cell r="K18">
+            <v>9.8000000000000007</v>
+          </cell>
+          <cell r="L18">
+            <v>11</v>
+          </cell>
+          <cell r="M18">
+            <v>11.1</v>
+          </cell>
+          <cell r="N18">
+            <v>11</v>
+          </cell>
+          <cell r="O18">
+            <v>11.6</v>
+          </cell>
+          <cell r="P18">
+            <v>12</v>
+          </cell>
+          <cell r="Q18">
+            <v>12.2</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="B19" t="str">
+            <v>All modes</v>
+          </cell>
+          <cell r="E19">
+            <v>67.8</v>
+          </cell>
+          <cell r="F19">
+            <v>69.7</v>
+          </cell>
+          <cell r="G19">
+            <v>68.400000000000006</v>
+          </cell>
+          <cell r="H19">
+            <v>62.2</v>
+          </cell>
+          <cell r="I19">
+            <v>60.5</v>
+          </cell>
+          <cell r="J19">
+            <v>67.5</v>
+          </cell>
+          <cell r="K19">
+            <v>64.400000000000006</v>
+          </cell>
+          <cell r="L19">
+            <v>63.5</v>
+          </cell>
+          <cell r="M19">
+            <v>64</v>
+          </cell>
+          <cell r="N19">
+            <v>60.2</v>
+          </cell>
+          <cell r="O19">
+            <v>60.21</v>
+          </cell>
+          <cell r="P19">
+            <v>61.921999999999997</v>
+          </cell>
+          <cell r="Q19">
+            <v>62.099999999999994</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="B22" t="str">
+            <v>Road 1</v>
+          </cell>
+          <cell r="E22">
+            <v>3.2</v>
+          </cell>
+          <cell r="F22">
+            <v>3.3</v>
+          </cell>
+          <cell r="G22">
+            <v>4.2</v>
+          </cell>
+          <cell r="H22">
+            <v>3.7</v>
+          </cell>
+          <cell r="I22">
+            <v>3.7</v>
+          </cell>
+          <cell r="J22">
+            <v>3.9</v>
+          </cell>
+          <cell r="K22">
+            <v>4</v>
+          </cell>
+          <cell r="L22">
+            <v>4.2</v>
+          </cell>
+          <cell r="M22">
+            <v>3.7</v>
+          </cell>
+          <cell r="N22">
+            <v>3.5</v>
+          </cell>
+          <cell r="O22">
+            <v>3.1</v>
+          </cell>
+          <cell r="P22">
+            <v>2.9</v>
+          </cell>
+          <cell r="Q22">
+            <v>2.7</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="B23" t="str">
+            <v xml:space="preserve">Rail </v>
+          </cell>
+          <cell r="E23">
+            <v>5.9</v>
+          </cell>
+          <cell r="F23">
+            <v>1.6</v>
+          </cell>
+          <cell r="G23">
+            <v>4.0999999999999996</v>
+          </cell>
+          <cell r="H23">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="I23">
+            <v>4.7</v>
+          </cell>
+          <cell r="J23">
+            <v>4.5999999999999996</v>
+          </cell>
+          <cell r="K23">
+            <v>4.8</v>
+          </cell>
+          <cell r="L23">
+            <v>5</v>
+          </cell>
+          <cell r="M23">
+            <v>5</v>
+          </cell>
+          <cell r="N23">
+            <v>5.4</v>
+          </cell>
+          <cell r="O23">
+            <v>3.9449999999999998</v>
+          </cell>
+          <cell r="P23">
+            <v>3.2719999999999998</v>
+          </cell>
+          <cell r="Q23">
+            <v>3.1</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="B24" t="str">
+            <v xml:space="preserve">Water </v>
+          </cell>
+          <cell r="E24">
+            <v>3.8</v>
+          </cell>
+          <cell r="F24">
+            <v>1.1000000000000001</v>
+          </cell>
+          <cell r="G24">
+            <v>3.1</v>
+          </cell>
+          <cell r="H24">
+            <v>3.7</v>
+          </cell>
+          <cell r="I24">
+            <v>2.9</v>
+          </cell>
+          <cell r="J24">
+            <v>2.9</v>
+          </cell>
+          <cell r="K24">
+            <v>2.6</v>
+          </cell>
+          <cell r="L24">
+            <v>1.4</v>
+          </cell>
+          <cell r="M24">
+            <v>1.8</v>
+          </cell>
+          <cell r="N24">
+            <v>1.8</v>
+          </cell>
+          <cell r="O24">
+            <v>1.5</v>
+          </cell>
+          <cell r="P24">
+            <v>1.4</v>
+          </cell>
+          <cell r="Q24">
+            <v>1.8</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="B25" t="str">
+            <v>All modes</v>
+          </cell>
+          <cell r="E25">
+            <v>12.900000000000002</v>
+          </cell>
+          <cell r="F25">
+            <v>6</v>
+          </cell>
+          <cell r="G25">
+            <v>11.4</v>
+          </cell>
+          <cell r="H25">
+            <v>12.5</v>
+          </cell>
+          <cell r="I25">
+            <v>11.3</v>
+          </cell>
+          <cell r="J25">
+            <v>11.4</v>
+          </cell>
+          <cell r="K25">
+            <v>11.4</v>
+          </cell>
+          <cell r="L25">
+            <v>10.6</v>
+          </cell>
+          <cell r="M25">
+            <v>10.5</v>
+          </cell>
+          <cell r="N25">
+            <v>10.700000000000001</v>
+          </cell>
+          <cell r="O25">
+            <v>8.5449999999999999</v>
+          </cell>
+          <cell r="P25">
+            <v>7.5719999999999992</v>
+          </cell>
+          <cell r="Q25">
+            <v>7.6000000000000005</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>Road 1</v>
+          </cell>
+          <cell r="E28">
+            <v>88.5</v>
+          </cell>
+          <cell r="F28">
+            <v>93.1</v>
+          </cell>
+          <cell r="G28">
+            <v>94.7</v>
+          </cell>
+          <cell r="H28">
+            <v>98</v>
+          </cell>
+          <cell r="I28">
+            <v>105.5</v>
+          </cell>
+          <cell r="J28">
+            <v>121.4</v>
+          </cell>
+          <cell r="K28">
+            <v>129.30000000000001</v>
+          </cell>
+          <cell r="L28">
+            <v>127.2</v>
+          </cell>
+          <cell r="M28">
+            <v>121.4</v>
+          </cell>
+          <cell r="N28">
+            <v>118.5</v>
+          </cell>
+          <cell r="O28">
+            <v>126.4</v>
+          </cell>
+          <cell r="P28">
+            <v>135.69999999999999</v>
+          </cell>
+          <cell r="Q28">
+            <v>141.19999999999999</v>
+          </cell>
+        </row>
+        <row r="29">
+          <cell r="B29" t="str">
+            <v xml:space="preserve">Rail </v>
+          </cell>
+          <cell r="E29">
+            <v>8.9</v>
+          </cell>
+          <cell r="F29">
+            <v>8.9</v>
+          </cell>
+          <cell r="G29">
+            <v>9.1999999999999993</v>
+          </cell>
+          <cell r="H29">
+            <v>9.4</v>
+          </cell>
+          <cell r="I29">
+            <v>10.6</v>
+          </cell>
+          <cell r="J29">
+            <v>11.4</v>
+          </cell>
+          <cell r="K29">
+            <v>10.3</v>
+          </cell>
+          <cell r="L29">
+            <v>8.6999999999999993</v>
+          </cell>
+          <cell r="M29">
+            <v>8.3000000000000007</v>
+          </cell>
+          <cell r="N29">
+            <v>8.1</v>
+          </cell>
+          <cell r="O29">
+            <v>7.91</v>
+          </cell>
+          <cell r="P29">
+            <v>7.8839999999999995</v>
+          </cell>
+          <cell r="Q29">
+            <v>8.5</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="B30" t="str">
+            <v xml:space="preserve">Water </v>
+          </cell>
+          <cell r="E30">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="F30">
+            <v>5.5</v>
+          </cell>
+          <cell r="G30">
+            <v>3.6</v>
+          </cell>
+          <cell r="H30">
+            <v>5.0999999999999996</v>
+          </cell>
+          <cell r="I30">
+            <v>7.3</v>
+          </cell>
+          <cell r="J30">
+            <v>7.1</v>
+          </cell>
+          <cell r="K30">
+            <v>7.4</v>
+          </cell>
+          <cell r="L30">
+            <v>8.6999999999999993</v>
+          </cell>
+          <cell r="M30">
+            <v>9.9</v>
+          </cell>
+          <cell r="N30">
+            <v>10.4</v>
+          </cell>
+          <cell r="O30">
+            <v>8</v>
+          </cell>
+          <cell r="P30">
+            <v>7.8</v>
+          </cell>
+          <cell r="Q30">
+            <v>8.3000000000000007</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="B31" t="str">
+            <v>All modes</v>
+          </cell>
+          <cell r="E31">
+            <v>102.5</v>
+          </cell>
+          <cell r="F31">
+            <v>107.5</v>
+          </cell>
+          <cell r="G31">
+            <v>107.5</v>
+          </cell>
+          <cell r="H31">
+            <v>112.5</v>
+          </cell>
+          <cell r="I31">
+            <v>123.39999999999999</v>
+          </cell>
+          <cell r="J31">
+            <v>139.9</v>
+          </cell>
+          <cell r="K31">
+            <v>147.00000000000003</v>
+          </cell>
+          <cell r="L31">
+            <v>144.6</v>
+          </cell>
+          <cell r="M31">
+            <v>139.60000000000002</v>
+          </cell>
+          <cell r="N31">
+            <v>137</v>
+          </cell>
+          <cell r="O31">
+            <v>142.31</v>
+          </cell>
+          <cell r="P31">
+            <v>151.38399999999999</v>
+          </cell>
+          <cell r="Q31">
+            <v>158</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="B34" t="str">
+            <v>Road 1</v>
+          </cell>
+          <cell r="E34">
+            <v>95.9</v>
+          </cell>
+          <cell r="F34">
+            <v>100.39999999999999</v>
+          </cell>
+          <cell r="G34">
+            <v>103.2</v>
+          </cell>
+          <cell r="H34">
+            <v>105.4</v>
+          </cell>
+          <cell r="I34">
+            <v>113.3</v>
+          </cell>
+          <cell r="J34">
+            <v>130.20000000000002</v>
+          </cell>
+          <cell r="K34">
+            <v>137.80000000000001</v>
+          </cell>
+          <cell r="L34">
+            <v>136.30000000000001</v>
+          </cell>
+          <cell r="M34">
+            <v>130</v>
+          </cell>
+          <cell r="N34">
+            <v>126.5</v>
+          </cell>
+          <cell r="O34">
+            <v>134.5</v>
+          </cell>
+          <cell r="P34">
+            <v>143.69999999999999</v>
+          </cell>
+          <cell r="Q34">
+            <v>149.6</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="B35" t="str">
+            <v xml:space="preserve">Rail </v>
+          </cell>
+          <cell r="E35">
+            <v>17.100000000000001</v>
+          </cell>
+          <cell r="F35">
+            <v>12.700000000000001</v>
+          </cell>
+          <cell r="G35">
+            <v>15.299999999999999</v>
+          </cell>
+          <cell r="H35">
+            <v>16.600000000000001</v>
+          </cell>
+          <cell r="I35">
+            <v>17.3</v>
+          </cell>
+          <cell r="J35">
+            <v>18.2</v>
+          </cell>
+          <cell r="K35">
+            <v>17.3</v>
+          </cell>
+          <cell r="L35">
+            <v>15.799999999999999</v>
+          </cell>
+          <cell r="M35">
+            <v>15.3</v>
+          </cell>
+          <cell r="N35">
+            <v>15.5</v>
+          </cell>
+          <cell r="O35">
+            <v>13.765000000000001</v>
+          </cell>
+          <cell r="P35">
+            <v>12.977999999999998</v>
+          </cell>
+          <cell r="Q35">
+            <v>13.3</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="B36" t="str">
+            <v xml:space="preserve">Water </v>
+          </cell>
+          <cell r="E36">
+            <v>60.3</v>
+          </cell>
+          <cell r="F36">
+            <v>59.7</v>
+          </cell>
+          <cell r="G36">
+            <v>57.6</v>
+          </cell>
+          <cell r="H36">
+            <v>54.800000000000004</v>
+          </cell>
+          <cell r="I36">
+            <v>54.099999999999994</v>
+          </cell>
+          <cell r="J36">
+            <v>59.3</v>
+          </cell>
+          <cell r="K36">
+            <v>57.9</v>
+          </cell>
+          <cell r="L36">
+            <v>55.7</v>
+          </cell>
+          <cell r="M36">
+            <v>57.699999999999996</v>
+          </cell>
+          <cell r="N36">
+            <v>54.900000000000006</v>
+          </cell>
+          <cell r="O36">
+            <v>51.2</v>
+          </cell>
+          <cell r="P36">
+            <v>52.2</v>
+          </cell>
+          <cell r="Q36">
+            <v>52.6</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="B37" t="str">
+            <v xml:space="preserve">Pipeline </v>
+          </cell>
+          <cell r="E37">
+            <v>9.9</v>
+          </cell>
+          <cell r="F37">
+            <v>10.4</v>
+          </cell>
+          <cell r="G37">
+            <v>11.2</v>
+          </cell>
+          <cell r="H37">
+            <v>10.4</v>
+          </cell>
+          <cell r="I37">
+            <v>10.5</v>
+          </cell>
+          <cell r="J37">
+            <v>11.1</v>
+          </cell>
+          <cell r="K37">
+            <v>9.8000000000000007</v>
+          </cell>
+          <cell r="L37">
+            <v>11</v>
+          </cell>
+          <cell r="M37">
+            <v>11.1</v>
+          </cell>
+          <cell r="N37">
+            <v>11</v>
+          </cell>
+          <cell r="O37">
+            <v>11.6</v>
+          </cell>
+          <cell r="P37">
+            <v>12</v>
+          </cell>
+          <cell r="Q37">
+            <v>12.2</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="B38" t="str">
+            <v xml:space="preserve">All modes </v>
+          </cell>
+          <cell r="E38">
+            <v>183.20000000000002</v>
+          </cell>
+          <cell r="F38">
+            <v>183.20000000000002</v>
+          </cell>
+          <cell r="G38">
+            <v>187.29999999999998</v>
+          </cell>
+          <cell r="H38">
+            <v>187.20000000000002</v>
+          </cell>
+          <cell r="I38">
+            <v>195.2</v>
+          </cell>
+          <cell r="J38">
+            <v>218.79999999999998</v>
+          </cell>
+          <cell r="K38">
+            <v>222.80000000000004</v>
+          </cell>
+          <cell r="L38">
+            <v>218.8</v>
+          </cell>
+          <cell r="M38">
+            <v>214.1</v>
+          </cell>
+          <cell r="N38">
+            <v>207.9</v>
+          </cell>
+          <cell r="O38">
+            <v>211.06499999999997</v>
+          </cell>
+          <cell r="P38">
+            <v>220.87799999999999</v>
+          </cell>
+          <cell r="Q38">
+            <v>227.7</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="B41" t="str">
+            <v>Road 1</v>
+          </cell>
+          <cell r="E41">
+            <v>52.3471615720524</v>
+          </cell>
+          <cell r="F41">
+            <v>54.803493449781648</v>
+          </cell>
+          <cell r="G41">
+            <v>55.098772023491726</v>
+          </cell>
+          <cell r="H41">
+            <v>56.303418803418801</v>
+          </cell>
+          <cell r="I41">
+            <v>58.043032786885249</v>
+          </cell>
+          <cell r="J41">
+            <v>59.506398537477153</v>
+          </cell>
+          <cell r="K41">
+            <v>61.849192100538595</v>
+          </cell>
+          <cell r="L41">
+            <v>62.294332723948806</v>
+          </cell>
+          <cell r="M41">
+            <v>60.719290051377861</v>
+          </cell>
+          <cell r="N41">
+            <v>60.846560846560848</v>
+          </cell>
+          <cell r="O41">
+            <v>63.724445076161388</v>
+          </cell>
+          <cell r="P41">
+            <v>65.058539103034249</v>
+          </cell>
+          <cell r="Q41">
+            <v>65.700483091787447</v>
+          </cell>
+        </row>
+        <row r="42">
+          <cell r="B42" t="str">
+            <v xml:space="preserve">Rail </v>
+          </cell>
+          <cell r="E42">
+            <v>9.3340611353711793</v>
+          </cell>
+          <cell r="F42">
+            <v>6.9323144104803491</v>
+          </cell>
+          <cell r="G42">
+            <v>8.1687132941804581</v>
+          </cell>
+          <cell r="H42">
+            <v>8.867521367521368</v>
+          </cell>
+          <cell r="I42">
+            <v>8.8627049180327884</v>
+          </cell>
+          <cell r="J42">
+            <v>8.3180987202925056</v>
+          </cell>
+          <cell r="K42">
+            <v>7.7648114901256724</v>
+          </cell>
+          <cell r="L42">
+            <v>7.221206581352833</v>
+          </cell>
+          <cell r="M42">
+            <v>7.1461933675852407</v>
+          </cell>
+          <cell r="N42">
+            <v>7.4555074555074556</v>
+          </cell>
+          <cell r="O42">
+            <v>6.5216876317722035</v>
+          </cell>
+          <cell r="P42">
+            <v>5.8756417569880197</v>
+          </cell>
+          <cell r="Q42">
+            <v>5.8410188844971467</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43" t="str">
+            <v xml:space="preserve">Water </v>
+          </cell>
+          <cell r="E43">
+            <v>32.914847161572048</v>
+          </cell>
+          <cell r="F43">
+            <v>32.587336244541483</v>
+          </cell>
+          <cell r="G43">
+            <v>30.752802989855848</v>
+          </cell>
+          <cell r="H43">
+            <v>29.273504273504276</v>
+          </cell>
+          <cell r="I43">
+            <v>27.715163934426229</v>
+          </cell>
+          <cell r="J43">
+            <v>27.102376599634368</v>
+          </cell>
+          <cell r="K43">
+            <v>25.987432675044879</v>
+          </cell>
+          <cell r="L43">
+            <v>25.457038391224863</v>
+          </cell>
+          <cell r="M43">
+            <v>26.950023353573094</v>
+          </cell>
+          <cell r="N43">
+            <v>26.406926406926406</v>
+          </cell>
+          <cell r="O43">
+            <v>24.257930021557346</v>
+          </cell>
+          <cell r="P43">
+            <v>23.632955749327685</v>
+          </cell>
+          <cell r="Q43">
+            <v>23.100570926657884</v>
+          </cell>
+        </row>
+        <row r="44">
+          <cell r="B44" t="str">
+            <v>Pipeline</v>
+          </cell>
+          <cell r="E44">
+            <v>5.4039301310043664</v>
+          </cell>
+          <cell r="F44">
+            <v>5.676855895196506</v>
+          </cell>
+          <cell r="G44">
+            <v>5.9797116924719704</v>
+          </cell>
+          <cell r="H44">
+            <v>5.5555555555555554</v>
+          </cell>
+          <cell r="I44">
+            <v>5.3790983606557381</v>
+          </cell>
+          <cell r="J44">
+            <v>5.0731261425959779</v>
+          </cell>
+          <cell r="K44">
+            <v>4.3985637342908435</v>
+          </cell>
+          <cell r="L44">
+            <v>5.0274223034734913</v>
+          </cell>
+          <cell r="M44">
+            <v>5.1844932274638014</v>
+          </cell>
+          <cell r="N44">
+            <v>5.2910052910052912</v>
+          </cell>
+          <cell r="O44">
+            <v>5.495937270509085</v>
+          </cell>
+          <cell r="P44">
+            <v>5.4328633906500423</v>
+          </cell>
+          <cell r="Q44">
+            <v>5.3579270970575319</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
       <sheetName val="CommentarySA"/>
       <sheetName val="TABLE1a"/>
       <sheetName val="TABLE1b"/>
@@ -1628,1111 +2747,6 @@
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink4.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="TIS-INDEX"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="9">
-          <cell r="E9">
-            <v>1983</v>
-          </cell>
-          <cell r="F9">
-            <v>1984</v>
-          </cell>
-          <cell r="G9">
-            <v>1985</v>
-          </cell>
-          <cell r="H9">
-            <v>1986</v>
-          </cell>
-          <cell r="I9">
-            <v>1987</v>
-          </cell>
-          <cell r="J9">
-            <v>1988</v>
-          </cell>
-          <cell r="K9">
-            <v>1989</v>
-          </cell>
-          <cell r="L9">
-            <v>1990</v>
-          </cell>
-          <cell r="M9">
-            <v>1991</v>
-          </cell>
-          <cell r="N9">
-            <v>1992</v>
-          </cell>
-          <cell r="O9">
-            <v>1993</v>
-          </cell>
-          <cell r="P9">
-            <v>1994</v>
-          </cell>
-          <cell r="Q9">
-            <v>1995</v>
-          </cell>
-          <cell r="R9">
-            <v>1996</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="B13" t="str">
-            <v>Road 1</v>
-          </cell>
-          <cell r="E13">
-            <v>4.2</v>
-          </cell>
-          <cell r="F13">
-            <v>4</v>
-          </cell>
-          <cell r="G13">
-            <v>4.3</v>
-          </cell>
-          <cell r="H13">
-            <v>3.7</v>
-          </cell>
-          <cell r="I13">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="J13">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="K13">
-            <v>4.5</v>
-          </cell>
-          <cell r="L13">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="M13">
-            <v>4.9000000000000004</v>
-          </cell>
-          <cell r="N13">
-            <v>4.5</v>
-          </cell>
-          <cell r="O13">
-            <v>5</v>
-          </cell>
-          <cell r="P13">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="Q13">
-            <v>5.7</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="B14" t="str">
-            <v xml:space="preserve">Rail </v>
-          </cell>
-          <cell r="E14">
-            <v>2.2999999999999998</v>
-          </cell>
-          <cell r="F14">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="G14">
-            <v>2</v>
-          </cell>
-          <cell r="H14">
-            <v>2.1</v>
-          </cell>
-          <cell r="I14">
-            <v>2</v>
-          </cell>
-          <cell r="J14">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="K14">
-            <v>2.2000000000000002</v>
-          </cell>
-          <cell r="L14">
-            <v>2.1</v>
-          </cell>
-          <cell r="M14">
-            <v>2</v>
-          </cell>
-          <cell r="N14">
-            <v>2</v>
-          </cell>
-          <cell r="O14">
-            <v>1.91</v>
-          </cell>
-          <cell r="P14">
-            <v>1.8220000000000001</v>
-          </cell>
-          <cell r="Q14">
-            <v>1.7</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="B15" t="str">
-            <v xml:space="preserve">Water </v>
-          </cell>
-          <cell r="E15">
-            <v>51.4</v>
-          </cell>
-          <cell r="F15">
-            <v>53.1</v>
-          </cell>
-          <cell r="G15">
-            <v>50.9</v>
-          </cell>
-          <cell r="H15">
-            <v>46</v>
-          </cell>
-          <cell r="I15">
-            <v>43.9</v>
-          </cell>
-          <cell r="J15">
-            <v>49.3</v>
-          </cell>
-          <cell r="K15">
-            <v>47.9</v>
-          </cell>
-          <cell r="L15">
-            <v>45.4</v>
-          </cell>
-          <cell r="M15">
-            <v>46</v>
-          </cell>
-          <cell r="N15">
-            <v>42.7</v>
-          </cell>
-          <cell r="O15">
-            <v>41.7</v>
-          </cell>
-          <cell r="P15">
-            <v>43</v>
-          </cell>
-          <cell r="Q15">
-            <v>42.5</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="B16" t="str">
-            <v>ow:  coastwise</v>
-          </cell>
-          <cell r="E16">
-            <v>40.200000000000003</v>
-          </cell>
-          <cell r="F16">
-            <v>41</v>
-          </cell>
-          <cell r="G16">
-            <v>38.9</v>
-          </cell>
-          <cell r="H16">
-            <v>33.9</v>
-          </cell>
-          <cell r="I16">
-            <v>31.4</v>
-          </cell>
-          <cell r="J16">
-            <v>34.200000000000003</v>
-          </cell>
-          <cell r="K16">
-            <v>34.1</v>
-          </cell>
-          <cell r="L16">
-            <v>32.1</v>
-          </cell>
-          <cell r="M16">
-            <v>31.2</v>
-          </cell>
-          <cell r="N16">
-            <v>29.4</v>
-          </cell>
-          <cell r="O16">
-            <v>28.9</v>
-          </cell>
-          <cell r="P16">
-            <v>28.9</v>
-          </cell>
-          <cell r="Q16">
-            <v>31.4</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="B17" t="str">
-            <v xml:space="preserve">Pipeline </v>
-          </cell>
-          <cell r="H17">
-            <v>10.4</v>
-          </cell>
-          <cell r="I17">
-            <v>10.5</v>
-          </cell>
-          <cell r="J17">
-            <v>11.1</v>
-          </cell>
-          <cell r="K17">
-            <v>9.8000000000000007</v>
-          </cell>
-          <cell r="L17">
-            <v>11.1</v>
-          </cell>
-          <cell r="M17">
-            <v>11.1</v>
-          </cell>
-          <cell r="N17">
-            <v>11</v>
-          </cell>
-          <cell r="O17">
-            <v>11.6</v>
-          </cell>
-          <cell r="P17">
-            <v>12</v>
-          </cell>
-          <cell r="Q17">
-            <v>12.2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="B18" t="str">
-            <v>Pipeline</v>
-          </cell>
-          <cell r="E18">
-            <v>9.9</v>
-          </cell>
-          <cell r="F18">
-            <v>10.4</v>
-          </cell>
-          <cell r="G18">
-            <v>11.2</v>
-          </cell>
-          <cell r="H18">
-            <v>10.4</v>
-          </cell>
-          <cell r="I18">
-            <v>10.5</v>
-          </cell>
-          <cell r="J18">
-            <v>11.1</v>
-          </cell>
-          <cell r="K18">
-            <v>9.8000000000000007</v>
-          </cell>
-          <cell r="L18">
-            <v>11</v>
-          </cell>
-          <cell r="M18">
-            <v>11.1</v>
-          </cell>
-          <cell r="N18">
-            <v>11</v>
-          </cell>
-          <cell r="O18">
-            <v>11.6</v>
-          </cell>
-          <cell r="P18">
-            <v>12</v>
-          </cell>
-          <cell r="Q18">
-            <v>12.2</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="B19" t="str">
-            <v>All modes</v>
-          </cell>
-          <cell r="E19">
-            <v>67.8</v>
-          </cell>
-          <cell r="F19">
-            <v>69.7</v>
-          </cell>
-          <cell r="G19">
-            <v>68.400000000000006</v>
-          </cell>
-          <cell r="H19">
-            <v>62.2</v>
-          </cell>
-          <cell r="I19">
-            <v>60.5</v>
-          </cell>
-          <cell r="J19">
-            <v>67.5</v>
-          </cell>
-          <cell r="K19">
-            <v>64.400000000000006</v>
-          </cell>
-          <cell r="L19">
-            <v>63.5</v>
-          </cell>
-          <cell r="M19">
-            <v>64</v>
-          </cell>
-          <cell r="N19">
-            <v>60.2</v>
-          </cell>
-          <cell r="O19">
-            <v>60.21</v>
-          </cell>
-          <cell r="P19">
-            <v>61.921999999999997</v>
-          </cell>
-          <cell r="Q19">
-            <v>62.099999999999994</v>
-          </cell>
-        </row>
-        <row r="22">
-          <cell r="B22" t="str">
-            <v>Road 1</v>
-          </cell>
-          <cell r="E22">
-            <v>3.2</v>
-          </cell>
-          <cell r="F22">
-            <v>3.3</v>
-          </cell>
-          <cell r="G22">
-            <v>4.2</v>
-          </cell>
-          <cell r="H22">
-            <v>3.7</v>
-          </cell>
-          <cell r="I22">
-            <v>3.7</v>
-          </cell>
-          <cell r="J22">
-            <v>3.9</v>
-          </cell>
-          <cell r="K22">
-            <v>4</v>
-          </cell>
-          <cell r="L22">
-            <v>4.2</v>
-          </cell>
-          <cell r="M22">
-            <v>3.7</v>
-          </cell>
-          <cell r="N22">
-            <v>3.5</v>
-          </cell>
-          <cell r="O22">
-            <v>3.1</v>
-          </cell>
-          <cell r="P22">
-            <v>2.9</v>
-          </cell>
-          <cell r="Q22">
-            <v>2.7</v>
-          </cell>
-        </row>
-        <row r="23">
-          <cell r="B23" t="str">
-            <v xml:space="preserve">Rail </v>
-          </cell>
-          <cell r="E23">
-            <v>5.9</v>
-          </cell>
-          <cell r="F23">
-            <v>1.6</v>
-          </cell>
-          <cell r="G23">
-            <v>4.0999999999999996</v>
-          </cell>
-          <cell r="H23">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="I23">
-            <v>4.7</v>
-          </cell>
-          <cell r="J23">
-            <v>4.5999999999999996</v>
-          </cell>
-          <cell r="K23">
-            <v>4.8</v>
-          </cell>
-          <cell r="L23">
-            <v>5</v>
-          </cell>
-          <cell r="M23">
-            <v>5</v>
-          </cell>
-          <cell r="N23">
-            <v>5.4</v>
-          </cell>
-          <cell r="O23">
-            <v>3.9449999999999998</v>
-          </cell>
-          <cell r="P23">
-            <v>3.2719999999999998</v>
-          </cell>
-          <cell r="Q23">
-            <v>3.1</v>
-          </cell>
-        </row>
-        <row r="24">
-          <cell r="B24" t="str">
-            <v xml:space="preserve">Water </v>
-          </cell>
-          <cell r="E24">
-            <v>3.8</v>
-          </cell>
-          <cell r="F24">
-            <v>1.1000000000000001</v>
-          </cell>
-          <cell r="G24">
-            <v>3.1</v>
-          </cell>
-          <cell r="H24">
-            <v>3.7</v>
-          </cell>
-          <cell r="I24">
-            <v>2.9</v>
-          </cell>
-          <cell r="J24">
-            <v>2.9</v>
-          </cell>
-          <cell r="K24">
-            <v>2.6</v>
-          </cell>
-          <cell r="L24">
-            <v>1.4</v>
-          </cell>
-          <cell r="M24">
-            <v>1.8</v>
-          </cell>
-          <cell r="N24">
-            <v>1.8</v>
-          </cell>
-          <cell r="O24">
-            <v>1.5</v>
-          </cell>
-          <cell r="P24">
-            <v>1.4</v>
-          </cell>
-          <cell r="Q24">
-            <v>1.8</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="B25" t="str">
-            <v>All modes</v>
-          </cell>
-          <cell r="E25">
-            <v>12.900000000000002</v>
-          </cell>
-          <cell r="F25">
-            <v>6</v>
-          </cell>
-          <cell r="G25">
-            <v>11.4</v>
-          </cell>
-          <cell r="H25">
-            <v>12.5</v>
-          </cell>
-          <cell r="I25">
-            <v>11.3</v>
-          </cell>
-          <cell r="J25">
-            <v>11.4</v>
-          </cell>
-          <cell r="K25">
-            <v>11.4</v>
-          </cell>
-          <cell r="L25">
-            <v>10.6</v>
-          </cell>
-          <cell r="M25">
-            <v>10.5</v>
-          </cell>
-          <cell r="N25">
-            <v>10.700000000000001</v>
-          </cell>
-          <cell r="O25">
-            <v>8.5449999999999999</v>
-          </cell>
-          <cell r="P25">
-            <v>7.5719999999999992</v>
-          </cell>
-          <cell r="Q25">
-            <v>7.6000000000000005</v>
-          </cell>
-        </row>
-        <row r="28">
-          <cell r="B28" t="str">
-            <v>Road 1</v>
-          </cell>
-          <cell r="E28">
-            <v>88.5</v>
-          </cell>
-          <cell r="F28">
-            <v>93.1</v>
-          </cell>
-          <cell r="G28">
-            <v>94.7</v>
-          </cell>
-          <cell r="H28">
-            <v>98</v>
-          </cell>
-          <cell r="I28">
-            <v>105.5</v>
-          </cell>
-          <cell r="J28">
-            <v>121.4</v>
-          </cell>
-          <cell r="K28">
-            <v>129.30000000000001</v>
-          </cell>
-          <cell r="L28">
-            <v>127.2</v>
-          </cell>
-          <cell r="M28">
-            <v>121.4</v>
-          </cell>
-          <cell r="N28">
-            <v>118.5</v>
-          </cell>
-          <cell r="O28">
-            <v>126.4</v>
-          </cell>
-          <cell r="P28">
-            <v>135.69999999999999</v>
-          </cell>
-          <cell r="Q28">
-            <v>141.19999999999999</v>
-          </cell>
-        </row>
-        <row r="29">
-          <cell r="B29" t="str">
-            <v xml:space="preserve">Rail </v>
-          </cell>
-          <cell r="E29">
-            <v>8.9</v>
-          </cell>
-          <cell r="F29">
-            <v>8.9</v>
-          </cell>
-          <cell r="G29">
-            <v>9.1999999999999993</v>
-          </cell>
-          <cell r="H29">
-            <v>9.4</v>
-          </cell>
-          <cell r="I29">
-            <v>10.6</v>
-          </cell>
-          <cell r="J29">
-            <v>11.4</v>
-          </cell>
-          <cell r="K29">
-            <v>10.3</v>
-          </cell>
-          <cell r="L29">
-            <v>8.6999999999999993</v>
-          </cell>
-          <cell r="M29">
-            <v>8.3000000000000007</v>
-          </cell>
-          <cell r="N29">
-            <v>8.1</v>
-          </cell>
-          <cell r="O29">
-            <v>7.91</v>
-          </cell>
-          <cell r="P29">
-            <v>7.8839999999999995</v>
-          </cell>
-          <cell r="Q29">
-            <v>8.5</v>
-          </cell>
-        </row>
-        <row r="30">
-          <cell r="B30" t="str">
-            <v xml:space="preserve">Water </v>
-          </cell>
-          <cell r="E30">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="F30">
-            <v>5.5</v>
-          </cell>
-          <cell r="G30">
-            <v>3.6</v>
-          </cell>
-          <cell r="H30">
-            <v>5.0999999999999996</v>
-          </cell>
-          <cell r="I30">
-            <v>7.3</v>
-          </cell>
-          <cell r="J30">
-            <v>7.1</v>
-          </cell>
-          <cell r="K30">
-            <v>7.4</v>
-          </cell>
-          <cell r="L30">
-            <v>8.6999999999999993</v>
-          </cell>
-          <cell r="M30">
-            <v>9.9</v>
-          </cell>
-          <cell r="N30">
-            <v>10.4</v>
-          </cell>
-          <cell r="O30">
-            <v>8</v>
-          </cell>
-          <cell r="P30">
-            <v>7.8</v>
-          </cell>
-          <cell r="Q30">
-            <v>8.3000000000000007</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="B31" t="str">
-            <v>All modes</v>
-          </cell>
-          <cell r="E31">
-            <v>102.5</v>
-          </cell>
-          <cell r="F31">
-            <v>107.5</v>
-          </cell>
-          <cell r="G31">
-            <v>107.5</v>
-          </cell>
-          <cell r="H31">
-            <v>112.5</v>
-          </cell>
-          <cell r="I31">
-            <v>123.39999999999999</v>
-          </cell>
-          <cell r="J31">
-            <v>139.9</v>
-          </cell>
-          <cell r="K31">
-            <v>147.00000000000003</v>
-          </cell>
-          <cell r="L31">
-            <v>144.6</v>
-          </cell>
-          <cell r="M31">
-            <v>139.60000000000002</v>
-          </cell>
-          <cell r="N31">
-            <v>137</v>
-          </cell>
-          <cell r="O31">
-            <v>142.31</v>
-          </cell>
-          <cell r="P31">
-            <v>151.38399999999999</v>
-          </cell>
-          <cell r="Q31">
-            <v>158</v>
-          </cell>
-        </row>
-        <row r="34">
-          <cell r="B34" t="str">
-            <v>Road 1</v>
-          </cell>
-          <cell r="E34">
-            <v>95.9</v>
-          </cell>
-          <cell r="F34">
-            <v>100.39999999999999</v>
-          </cell>
-          <cell r="G34">
-            <v>103.2</v>
-          </cell>
-          <cell r="H34">
-            <v>105.4</v>
-          </cell>
-          <cell r="I34">
-            <v>113.3</v>
-          </cell>
-          <cell r="J34">
-            <v>130.20000000000002</v>
-          </cell>
-          <cell r="K34">
-            <v>137.80000000000001</v>
-          </cell>
-          <cell r="L34">
-            <v>136.30000000000001</v>
-          </cell>
-          <cell r="M34">
-            <v>130</v>
-          </cell>
-          <cell r="N34">
-            <v>126.5</v>
-          </cell>
-          <cell r="O34">
-            <v>134.5</v>
-          </cell>
-          <cell r="P34">
-            <v>143.69999999999999</v>
-          </cell>
-          <cell r="Q34">
-            <v>149.6</v>
-          </cell>
-        </row>
-        <row r="35">
-          <cell r="B35" t="str">
-            <v xml:space="preserve">Rail </v>
-          </cell>
-          <cell r="E35">
-            <v>17.100000000000001</v>
-          </cell>
-          <cell r="F35">
-            <v>12.700000000000001</v>
-          </cell>
-          <cell r="G35">
-            <v>15.299999999999999</v>
-          </cell>
-          <cell r="H35">
-            <v>16.600000000000001</v>
-          </cell>
-          <cell r="I35">
-            <v>17.3</v>
-          </cell>
-          <cell r="J35">
-            <v>18.2</v>
-          </cell>
-          <cell r="K35">
-            <v>17.3</v>
-          </cell>
-          <cell r="L35">
-            <v>15.799999999999999</v>
-          </cell>
-          <cell r="M35">
-            <v>15.3</v>
-          </cell>
-          <cell r="N35">
-            <v>15.5</v>
-          </cell>
-          <cell r="O35">
-            <v>13.765000000000001</v>
-          </cell>
-          <cell r="P35">
-            <v>12.977999999999998</v>
-          </cell>
-          <cell r="Q35">
-            <v>13.3</v>
-          </cell>
-        </row>
-        <row r="36">
-          <cell r="B36" t="str">
-            <v xml:space="preserve">Water </v>
-          </cell>
-          <cell r="E36">
-            <v>60.3</v>
-          </cell>
-          <cell r="F36">
-            <v>59.7</v>
-          </cell>
-          <cell r="G36">
-            <v>57.6</v>
-          </cell>
-          <cell r="H36">
-            <v>54.800000000000004</v>
-          </cell>
-          <cell r="I36">
-            <v>54.099999999999994</v>
-          </cell>
-          <cell r="J36">
-            <v>59.3</v>
-          </cell>
-          <cell r="K36">
-            <v>57.9</v>
-          </cell>
-          <cell r="L36">
-            <v>55.7</v>
-          </cell>
-          <cell r="M36">
-            <v>57.699999999999996</v>
-          </cell>
-          <cell r="N36">
-            <v>54.900000000000006</v>
-          </cell>
-          <cell r="O36">
-            <v>51.2</v>
-          </cell>
-          <cell r="P36">
-            <v>52.2</v>
-          </cell>
-          <cell r="Q36">
-            <v>52.6</v>
-          </cell>
-        </row>
-        <row r="37">
-          <cell r="B37" t="str">
-            <v xml:space="preserve">Pipeline </v>
-          </cell>
-          <cell r="E37">
-            <v>9.9</v>
-          </cell>
-          <cell r="F37">
-            <v>10.4</v>
-          </cell>
-          <cell r="G37">
-            <v>11.2</v>
-          </cell>
-          <cell r="H37">
-            <v>10.4</v>
-          </cell>
-          <cell r="I37">
-            <v>10.5</v>
-          </cell>
-          <cell r="J37">
-            <v>11.1</v>
-          </cell>
-          <cell r="K37">
-            <v>9.8000000000000007</v>
-          </cell>
-          <cell r="L37">
-            <v>11</v>
-          </cell>
-          <cell r="M37">
-            <v>11.1</v>
-          </cell>
-          <cell r="N37">
-            <v>11</v>
-          </cell>
-          <cell r="O37">
-            <v>11.6</v>
-          </cell>
-          <cell r="P37">
-            <v>12</v>
-          </cell>
-          <cell r="Q37">
-            <v>12.2</v>
-          </cell>
-        </row>
-        <row r="38">
-          <cell r="B38" t="str">
-            <v xml:space="preserve">All modes </v>
-          </cell>
-          <cell r="E38">
-            <v>183.20000000000002</v>
-          </cell>
-          <cell r="F38">
-            <v>183.20000000000002</v>
-          </cell>
-          <cell r="G38">
-            <v>187.29999999999998</v>
-          </cell>
-          <cell r="H38">
-            <v>187.20000000000002</v>
-          </cell>
-          <cell r="I38">
-            <v>195.2</v>
-          </cell>
-          <cell r="J38">
-            <v>218.79999999999998</v>
-          </cell>
-          <cell r="K38">
-            <v>222.80000000000004</v>
-          </cell>
-          <cell r="L38">
-            <v>218.8</v>
-          </cell>
-          <cell r="M38">
-            <v>214.1</v>
-          </cell>
-          <cell r="N38">
-            <v>207.9</v>
-          </cell>
-          <cell r="O38">
-            <v>211.06499999999997</v>
-          </cell>
-          <cell r="P38">
-            <v>220.87799999999999</v>
-          </cell>
-          <cell r="Q38">
-            <v>227.7</v>
-          </cell>
-        </row>
-        <row r="41">
-          <cell r="B41" t="str">
-            <v>Road 1</v>
-          </cell>
-          <cell r="E41">
-            <v>52.3471615720524</v>
-          </cell>
-          <cell r="F41">
-            <v>54.803493449781648</v>
-          </cell>
-          <cell r="G41">
-            <v>55.098772023491726</v>
-          </cell>
-          <cell r="H41">
-            <v>56.303418803418801</v>
-          </cell>
-          <cell r="I41">
-            <v>58.043032786885249</v>
-          </cell>
-          <cell r="J41">
-            <v>59.506398537477153</v>
-          </cell>
-          <cell r="K41">
-            <v>61.849192100538595</v>
-          </cell>
-          <cell r="L41">
-            <v>62.294332723948806</v>
-          </cell>
-          <cell r="M41">
-            <v>60.719290051377861</v>
-          </cell>
-          <cell r="N41">
-            <v>60.846560846560848</v>
-          </cell>
-          <cell r="O41">
-            <v>63.724445076161388</v>
-          </cell>
-          <cell r="P41">
-            <v>65.058539103034249</v>
-          </cell>
-          <cell r="Q41">
-            <v>65.700483091787447</v>
-          </cell>
-        </row>
-        <row r="42">
-          <cell r="B42" t="str">
-            <v xml:space="preserve">Rail </v>
-          </cell>
-          <cell r="E42">
-            <v>9.3340611353711793</v>
-          </cell>
-          <cell r="F42">
-            <v>6.9323144104803491</v>
-          </cell>
-          <cell r="G42">
-            <v>8.1687132941804581</v>
-          </cell>
-          <cell r="H42">
-            <v>8.867521367521368</v>
-          </cell>
-          <cell r="I42">
-            <v>8.8627049180327884</v>
-          </cell>
-          <cell r="J42">
-            <v>8.3180987202925056</v>
-          </cell>
-          <cell r="K42">
-            <v>7.7648114901256724</v>
-          </cell>
-          <cell r="L42">
-            <v>7.221206581352833</v>
-          </cell>
-          <cell r="M42">
-            <v>7.1461933675852407</v>
-          </cell>
-          <cell r="N42">
-            <v>7.4555074555074556</v>
-          </cell>
-          <cell r="O42">
-            <v>6.5216876317722035</v>
-          </cell>
-          <cell r="P42">
-            <v>5.8756417569880197</v>
-          </cell>
-          <cell r="Q42">
-            <v>5.8410188844971467</v>
-          </cell>
-        </row>
-        <row r="43">
-          <cell r="B43" t="str">
-            <v xml:space="preserve">Water </v>
-          </cell>
-          <cell r="E43">
-            <v>32.914847161572048</v>
-          </cell>
-          <cell r="F43">
-            <v>32.587336244541483</v>
-          </cell>
-          <cell r="G43">
-            <v>30.752802989855848</v>
-          </cell>
-          <cell r="H43">
-            <v>29.273504273504276</v>
-          </cell>
-          <cell r="I43">
-            <v>27.715163934426229</v>
-          </cell>
-          <cell r="J43">
-            <v>27.102376599634368</v>
-          </cell>
-          <cell r="K43">
-            <v>25.987432675044879</v>
-          </cell>
-          <cell r="L43">
-            <v>25.457038391224863</v>
-          </cell>
-          <cell r="M43">
-            <v>26.950023353573094</v>
-          </cell>
-          <cell r="N43">
-            <v>26.406926406926406</v>
-          </cell>
-          <cell r="O43">
-            <v>24.257930021557346</v>
-          </cell>
-          <cell r="P43">
-            <v>23.632955749327685</v>
-          </cell>
-          <cell r="Q43">
-            <v>23.100570926657884</v>
-          </cell>
-        </row>
-        <row r="44">
-          <cell r="B44" t="str">
-            <v>Pipeline</v>
-          </cell>
-          <cell r="E44">
-            <v>5.4039301310043664</v>
-          </cell>
-          <cell r="F44">
-            <v>5.676855895196506</v>
-          </cell>
-          <cell r="G44">
-            <v>5.9797116924719704</v>
-          </cell>
-          <cell r="H44">
-            <v>5.5555555555555554</v>
-          </cell>
-          <cell r="I44">
-            <v>5.3790983606557381</v>
-          </cell>
-          <cell r="J44">
-            <v>5.0731261425959779</v>
-          </cell>
-          <cell r="K44">
-            <v>4.3985637342908435</v>
-          </cell>
-          <cell r="L44">
-            <v>5.0274223034734913</v>
-          </cell>
-          <cell r="M44">
-            <v>5.1844932274638014</v>
-          </cell>
-          <cell r="N44">
-            <v>5.2910052910052912</v>
-          </cell>
-          <cell r="O44">
-            <v>5.495937270509085</v>
-          </cell>
-          <cell r="P44">
-            <v>5.4328633906500423</v>
-          </cell>
-          <cell r="Q44">
-            <v>5.3579270970575319</v>
-          </cell>
-        </row>
-      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3003,8 +3017,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B11:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -3082,11 +3096,12 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="21" spans="2:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="B21" s="19" t="str">
-        <f>HYPERLINK("[TRA2501]TRA2501a!A1","TRA2501a")</f>
+    <row r="21" spans="2:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="str">
+        <f>HYPERLINK("#TRA2501a!A1","TRA2501a")</f>
         <v>TRA2501a</v>
       </c>
+      <c r="C21" s="17"/>
       <c r="E21" s="5" t="s">
         <v>7</v>
       </c>
@@ -3097,8 +3112,8 @@
       <c r="J21" s="5"/>
     </row>
     <row r="22" spans="2:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="B22" s="19" t="str">
-        <f>HYPERLINK("[TRA2501]TRA2501b!A1","TRA2501b")</f>
+      <c r="B22" s="20" t="str">
+        <f>HYPERLINK("#TRA2501b!A1","TRA2501b")</f>
         <v>TRA2501b</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -3111,8 +3126,8 @@
       <c r="J22" s="5"/>
     </row>
     <row r="23" spans="2:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="B23" s="19" t="str">
-        <f>HYPERLINK("[TRA2501]TRA2501c!A1","TRA2501c")</f>
+      <c r="B23" s="20" t="str">
+        <f>HYPERLINK("#TRA2501c!A1","TRA2501c")</f>
         <v>TRA2501c</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -3125,9 +3140,9 @@
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="2:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="B24" s="19" t="str">
-        <f t="shared" ref="B22:B27" si="0">HYPERLINK("[TRA2501]TRA2501a!A1","TRA2501a")</f>
-        <v>TRA2501a</v>
+      <c r="B24" s="20" t="str">
+        <f>HYPERLINK("#TRA2501d!A1","TRA2501d")</f>
+        <v>TRA2501d</v>
       </c>
       <c r="E24" s="5" t="s">
         <v>10</v>
@@ -3146,9 +3161,9 @@
       <c r="Q24" s="5"/>
     </row>
     <row r="25" spans="2:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="B25" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>TRA2501a</v>
+      <c r="B25" s="20" t="str">
+        <f>HYPERLINK("#TRA2501e!A1","TRA2501e")</f>
+        <v>TRA2501e</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>11</v>
@@ -3167,9 +3182,9 @@
       <c r="Q25" s="5"/>
     </row>
     <row r="26" spans="2:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="B26" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>TRA2501a</v>
+      <c r="B26" s="20" t="str">
+        <f>HYPERLINK("#TRA2501f!A1","TRA2501f")</f>
+        <v>TRA2501f</v>
       </c>
       <c r="E26" s="5" t="s">
         <v>12</v>
@@ -3188,9 +3203,9 @@
       <c r="Q26" s="5"/>
     </row>
     <row r="27" spans="2:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="B27" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v>TRA2501a</v>
+      <c r="B27" s="20" t="str">
+        <f>HYPERLINK("#TRA2501g!A1","TRA2501g")</f>
+        <v>TRA2501g</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>13</v>
@@ -3202,7 +3217,7 @@
       <c r="J27" s="5"/>
     </row>
     <row r="28" spans="2:26" ht="15" x14ac:dyDescent="0.2">
-      <c r="B28" s="5"/>
+      <c r="B28" s="21"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
       <c r="E28" s="12"/>
@@ -3249,20 +3264,20 @@
       <c r="B31" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E31" s="17" t="s">
+      <c r="E31" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-      <c r="M31" s="17"/>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="18"/>
+      <c r="I31" s="18"/>
+      <c r="J31" s="18"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="18"/>
+      <c r="O31" s="18"/>
+      <c r="P31" s="18"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
       <c r="S31" s="5"/>
@@ -3278,19 +3293,19 @@
       <c r="B32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E32" s="18" t="s">
+      <c r="E32" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
       <c r="P32" s="13"/>
       <c r="Q32" s="13"/>
       <c r="R32" s="13"/>
@@ -3307,17 +3322,17 @@
       <c r="B33" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="18"/>
-      <c r="F33" s="18"/>
-      <c r="G33" s="18"/>
-      <c r="H33" s="18"/>
-      <c r="I33" s="18"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="18"/>
-      <c r="L33" s="18"/>
-      <c r="M33" s="18"/>
-      <c r="N33" s="18"/>
-      <c r="O33" s="18"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
       <c r="P33" s="14"/>
       <c r="Q33" s="14"/>
       <c r="R33" s="14"/>
@@ -3411,11 +3426,9 @@
     <mergeCell ref="E32:O33"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B21" location="TRA2501a!A1" display="TRA2501a"/>
     <hyperlink ref="E31" r:id="rId1"/>
     <hyperlink ref="E32" r:id="rId2"/>
     <hyperlink ref="M38" r:id="rId3"/>
-    <hyperlink ref="B22:B27" location="TRA2501a!A1" display="TRA2501a"/>
   </hyperlinks>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" scale="64" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId4"/>

</xml_diff>